<commit_message>
CQ functionaly test for kudo complaint and delete
</commit_message>
<xml_diff>
--- a/resources/CQ.xlsx
+++ b/resources/CQ.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27907"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kavya.mothukuri/work_repos/ironman-qa-repo/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="28455" windowHeight="13005"/>
+    <workbookView xWindow="31200" yWindow="2360" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="kudo" sheetId="1" r:id="rId1"/>
+    <sheet name="complain" sheetId="2" r:id="rId2"/>
+    <sheet name="delete" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -69,9 +82,6 @@
     <t>input</t>
   </si>
   <si>
-    <t xml:space="preserve">20170323011952 </t>
-  </si>
-  <si>
     <t>/html/body/div/div/md-content/div/md-content/md-virtual-repeat-container/div/div[2]/md-list-item[1]/div/button</t>
   </si>
   <si>
@@ -148,13 +158,73 @@
   </si>
   <si>
     <t>escape</t>
+  </si>
+  <si>
+    <t>patient</t>
+  </si>
+  <si>
+    <t>//md-list-item/div/button</t>
+  </si>
+  <si>
+    <t>Click add icon</t>
+  </si>
+  <si>
+    <t>Add kudo</t>
+  </si>
+  <si>
+    <t>Add details</t>
+  </si>
+  <si>
+    <t>contact status</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>Jody</t>
+  </si>
+  <si>
+    <t>NO REMARKS</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/div/div/md-content/md-content/md-content[1]/md-fab-speed-dial/md-fab-actions/div[2]/button</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-fab-speed-dial/md-fab-trigger</t>
+  </si>
+  <si>
+    <t>//div[@id='widget']/div/div/div/div/p/span</t>
+  </si>
+  <si>
+    <t>//md-radio-button/div/div</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/md-content/form/md-input-container[2]/textarea</t>
+  </si>
+  <si>
+    <t>//div[3]/md-select-menu/md-content/md-option[3]/div</t>
+  </si>
+  <si>
+    <t>//md-toolbar[2]/button[2]</t>
+  </si>
+  <si>
+    <t>//md-input-container[4]/md-select</t>
+  </si>
+  <si>
+    <t>//md-option[2]/div[2]</t>
+  </si>
+  <si>
+    <t>//md-autocomplete-parent-scope/span</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +283,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -259,12 +334,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -291,14 +366,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -325,6 +401,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,27 +577,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:G18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35.5703125" defaultRowHeight="25.5" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="35.5" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="3"/>
-    <col min="2" max="2" width="50.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="35.5703125" style="4"/>
-    <col min="5" max="5" width="9.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="35.5703125" style="3"/>
+    <col min="1" max="1" width="35.5" style="3"/>
+    <col min="2" max="2" width="50.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="35.5" style="4"/>
+    <col min="5" max="5" width="9.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="35.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" customHeight="1">
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.5" customHeight="1">
+    <row r="2" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -563,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="25.5" customHeight="1">
+    <row r="3" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -583,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="25.5" customHeight="1">
+    <row r="4" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -603,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="25.5" customHeight="1">
+    <row r="5" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -614,15 +691,21 @@
         <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="25.5" customHeight="1">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -637,15 +720,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="25.5" customHeight="1">
+    <row r="7" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -657,12 +740,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="25.5" customHeight="1">
+    <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -677,9 +760,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="25.5" customHeight="1">
+    <row r="9" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -694,9 +780,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="25.5" customHeight="1">
+    <row r="10" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -711,26 +800,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="25.5" customHeight="1">
+    <row r="11" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="25.5" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
@@ -745,75 +834,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>28</v>
+    <row r="13" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="25.5" customHeight="1">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="25.5" customHeight="1">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="25.5" customHeight="1">
-      <c r="B17" s="6" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="3">
         <v>1</v>
       </c>
@@ -824,12 +920,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="25.5" customHeight="1">
+    <row r="18" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>9</v>
@@ -841,49 +937,6 @@
         <v>1</v>
       </c>
       <c r="G18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3">
         <v>1</v>
       </c>
     </row>
@@ -894,24 +947,299 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="3">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added delete and other functionalities
</commit_message>
<xml_diff>
--- a/resources/CQ.xlsx
+++ b/resources/CQ.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31200" yWindow="2360" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="kudo" sheetId="1" r:id="rId1"/>
-    <sheet name="complain" sheetId="2" r:id="rId2"/>
+    <sheet name="complain" sheetId="2" r:id="rId1"/>
+    <sheet name="kudo" sheetId="1" r:id="rId2"/>
     <sheet name="delete" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -82,142 +82,247 @@
     <t>input</t>
   </si>
   <si>
-    <t>/html/body/div/div/md-content/div/md-content/md-virtual-repeat-container/div/div[2]/md-list-item[1]/div/button</t>
-  </si>
-  <si>
     <t>Click First Patient</t>
   </si>
   <si>
-    <t>(//div[@id="widget" and @class="timeline-widget margin-0 flex-70 flex-xs-100  widget md-whiteframe-z2 widget md-whiteframe-z2 flex-order-1 layout-column flex"])[2]</t>
-  </si>
-  <si>
-    <t>day 1 - 3 call</t>
-  </si>
-  <si>
-    <t>//md-radio-group[@ng-model="vm.log.status.contactStatus"]//md-radio-button[1]</t>
-  </si>
-  <si>
-    <t>spoke with patient</t>
-  </si>
-  <si>
-    <t>//md-radio-group[@ng-model="vm.log.followups[0].idBadgeWorn"]//md-radio-button[1]</t>
-  </si>
-  <si>
-    <t>//md-radio-group[@ng-model="vm.log.followups[0].explainedHHAndServices"]//md-radio-button[1]</t>
-  </si>
-  <si>
-    <t>//md-radio-group[@ng-model="vm.log.followups[0].socPacketReceived"]//md-radio-button[1]</t>
-  </si>
-  <si>
-    <t>//md-radio-group[@ng-model="vm.log.followups[0].fluVaccine"]//md-radio-button[1]</t>
-  </si>
-  <si>
-    <t>//textarea[@ng-model="vm.log.followups[0].note"]</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>//textarea[@ng-model="vm.log.followups[vm.isKudo].receiveBy"]</t>
-  </si>
-  <si>
-    <t>//textarea[@ng-model="vm.log.followups[vm.isKudo].agency"]</t>
-  </si>
-  <si>
-    <t>receive by</t>
+    <t>//input[@name="admittingClinician"]</t>
+  </si>
+  <si>
+    <t>nature of kudo</t>
+  </si>
+  <si>
+    <t>main person involved</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>/html/body/md-backdrop</t>
+  </si>
+  <si>
+    <t>escape</t>
+  </si>
+  <si>
+    <t>patient</t>
+  </si>
+  <si>
+    <t>//md-list-item/div/button</t>
+  </si>
+  <si>
+    <t>Click add icon</t>
+  </si>
+  <si>
+    <t>Add kudo</t>
+  </si>
+  <si>
+    <t>Add details</t>
+  </si>
+  <si>
+    <t>contact status</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>Jody</t>
+  </si>
+  <si>
+    <t>NO REMARKS</t>
+  </si>
+  <si>
+    <t>/html/body/div/div/md-content/div/div/md-content/md-content/md-content[1]/md-fab-speed-dial/md-fab-actions/div[2]/button</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-fab-speed-dial/md-fab-trigger</t>
+  </si>
+  <si>
+    <t>//div[@id='widget']/div/div/div/div/p/span</t>
+  </si>
+  <si>
+    <t>//md-radio-button/div/div</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/md-content/form/md-input-container[2]/textarea</t>
+  </si>
+  <si>
+    <t>//div[3]/md-select-menu/md-content/md-option[3]/div</t>
+  </si>
+  <si>
+    <t>//md-toolbar[2]/button[2]</t>
+  </si>
+  <si>
+    <t>//md-input-container[4]/md-select</t>
+  </si>
+  <si>
+    <t>//md-option[2]/div[2]</t>
+  </si>
+  <si>
+    <t>//md-autocomplete-parent-scope/span</t>
+  </si>
+  <si>
+    <t>select complain</t>
+  </si>
+  <si>
+    <t>remarks for complaint</t>
+  </si>
+  <si>
+    <t>Employee receiving call</t>
   </si>
   <si>
     <t>agency</t>
   </si>
   <si>
-    <t>//md-select[@ng-model="vm.log.followups[vm.isKudo].kudoNature"]</t>
-  </si>
-  <si>
-    <t>//div[@class="_md-select-menu-container md-cs-content-theme-theme _md-active _md-clickable"]//md-option[1]</t>
-  </si>
-  <si>
-    <t>//input[@name="admittingClinician"]</t>
-  </si>
-  <si>
-    <t>admittingClinician</t>
-  </si>
-  <si>
-    <t>nature of kudo</t>
-  </si>
-  <si>
-    <t>main person involved</t>
-  </si>
-  <si>
-    <t>//*[@id="ui-admin-email"]/md-content/md-content/md-toolbar[2]/button</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>/html/body/md-backdrop</t>
-  </si>
-  <si>
-    <t>escape</t>
-  </si>
-  <si>
-    <t>patient</t>
-  </si>
-  <si>
-    <t>//md-list-item/div/button</t>
-  </si>
-  <si>
-    <t>Click add icon</t>
-  </si>
-  <si>
-    <t>Add kudo</t>
-  </si>
-  <si>
-    <t>Add details</t>
-  </si>
-  <si>
-    <t>contact status</t>
-  </si>
-  <si>
-    <t>remarks</t>
-  </si>
-  <si>
-    <t>Jody</t>
-  </si>
-  <si>
-    <t>NO REMARKS</t>
-  </si>
-  <si>
-    <t>/html/body/div/div/md-content/div/div/md-content/md-content/md-content[1]/md-fab-speed-dial/md-fab-actions/div[2]/button</t>
-  </si>
-  <si>
-    <t>hover</t>
-  </si>
-  <si>
-    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-fab-speed-dial/md-fab-trigger</t>
-  </si>
-  <si>
-    <t>//div[@id='widget']/div/div/div/div/p/span</t>
-  </si>
-  <si>
-    <t>//md-radio-button/div/div</t>
-  </si>
-  <si>
-    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/md-content/form/md-input-container[2]/textarea</t>
-  </si>
-  <si>
-    <t>//div[3]/md-select-menu/md-content/md-option[3]/div</t>
-  </si>
-  <si>
-    <t>//md-toolbar[2]/button[2]</t>
-  </si>
-  <si>
-    <t>//md-input-container[4]/md-select</t>
-  </si>
-  <si>
-    <t>//md-option[2]/div[2]</t>
-  </si>
-  <si>
-    <t>//md-autocomplete-parent-scope/span</t>
+    <t>kaiser</t>
+  </si>
+  <si>
+    <t>recived</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[2]/textarea</t>
+  </si>
+  <si>
+    <t>//div[3]/md-select-menu/md-content/md-option[5]/div</t>
+  </si>
+  <si>
+    <t>//div[3]/md-select-menu/md-content/md-option[6]/div</t>
+  </si>
+  <si>
+    <t>//div[3]/md-select-menu/md-content/md-option[7]/div</t>
+  </si>
+  <si>
+    <t>//div[3]/md-select-menu/md-content/md-option[10]/div</t>
+  </si>
+  <si>
+    <t>//input[@name="Clinician"]</t>
+  </si>
+  <si>
+    <t>mandy</t>
+  </si>
+  <si>
+    <t>//div[2]/ul/li</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>no propercare</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Reviewed mgr</t>
+  </si>
+  <si>
+    <t>Maya Myra</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>dept chief</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Reviewed Dept chief</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Dept chief</t>
+  </si>
+  <si>
+    <t>Audit dept</t>
+  </si>
+  <si>
+    <t>Mgr report</t>
+  </si>
+  <si>
+    <t>Inprogress</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[5]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[6]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[7]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[8]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[9]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[10]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[11]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[12]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[13]/textarea</t>
+  </si>
+  <si>
+    <t>//md-content[@id='ui-admin-email']/md-content/md-content/md-dialog-content/md-content/div[3]/md-content/form/md-input-container[14]/textarea</t>
+  </si>
+  <si>
+    <t>//md-fab-actions/div/button</t>
+  </si>
+  <si>
+    <t>patr</t>
+  </si>
+  <si>
+    <t>//md-radio-button[3]</t>
+  </si>
+  <si>
+    <t>//md-dialog-actions/button[2]</t>
+  </si>
+  <si>
+    <t>confirm delete</t>
+  </si>
+  <si>
+    <t>//md-toolbar[2]/button</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>//md-dialog-actions/button</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>mar</t>
   </si>
 </sst>
 </file>
@@ -578,10 +683,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="35.5" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -691,7 +1375,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -702,10 +1386,10 @@
     </row>
     <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -722,13 +1406,13 @@
     </row>
     <row r="7" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -742,10 +1426,10 @@
     </row>
     <row r="8" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
@@ -762,10 +1446,10 @@
     </row>
     <row r="9" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>9</v>
@@ -782,10 +1466,10 @@
     </row>
     <row r="10" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -802,24 +1486,24 @@
     </row>
     <row r="11" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
@@ -836,7 +1520,7 @@
     </row>
     <row r="13" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
@@ -853,7 +1537,7 @@
     </row>
     <row r="14" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>9</v>
@@ -870,10 +1554,10 @@
     </row>
     <row r="15" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>9</v>
@@ -890,21 +1574,21 @@
     </row>
     <row r="16" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>9</v>
@@ -922,10 +1606,10 @@
     </row>
     <row r="18" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>9</v>
@@ -946,48 +1630,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="67.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -1003,9 +1688,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -1021,9 +1709,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -1039,27 +1730,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -1075,54 +1771,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>94</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -1138,9 +1855,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
-        <v>34</v>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
@@ -1156,12 +1876,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
@@ -1177,19 +1897,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D13" s="4"/>
       <c r="E13" s="3">
         <v>1</v>
       </c>
@@ -1200,47 +1918,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>